<commit_message>
updates to wayside controller
</commit_message>
<xml_diff>
--- a/src/WaysideController/TrackBlockData.xlsx
+++ b/src/WaysideController/TrackBlockData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsant\Repos\1140\src\WaysideController\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\japro\OneDrive\Documents2\Pitt\Systems &amp; Project Engineering\2021 Summer Term\Lectures\Lecture 2 - Project\Project Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CD4829C-403F-4928-A736-48BA99AB438F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28548DF3-BD3E-4F62-BE50-9FA9D7A0FF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5800" yWindow="-21710" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -566,8 +566,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="37440" y="4080910"/>
-          <a:ext cx="6907750" cy="2580640"/>
+          <a:off x="37440" y="4166952"/>
+          <a:ext cx="7275415" cy="2600008"/>
           <a:chOff x="37440" y="4060590"/>
           <a:chExt cx="6967440" cy="2598420"/>
         </a:xfrm>
@@ -1219,16 +1219,16 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1539 3233,'281'0,"-268"1,0 0,24 6,-23-4,-1 0,20 0,418-1,-221-4,-37 2,-179 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2111.37">3166 3251,'1313'0,"-1299"0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3690.33">4967 3233,'1189'0,"-1173"0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5880.65">6627 3215,'1133'0,"-1120"1,-1 0,25 6,13 2,-36-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8698.84">0 3215,'559'0,"-543"1,0 0,22 6,-20-3,-2-2,21 2,12-5,-23 0,-2 1,2 1,-1 2,25 5,-23-4,1 0,0-2,-1-1,37-3,0 0,6 2,-55 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14544.8">8429 3058,'6'-1,"0"0,-1 0,0-1,1 0,-1 0,-1 0,2-1,-1 1,0-1,-1 0,2-1,4-5,-5 4,3 0,-3 1,2 0,0 0,0 2,7-5,21-5,-2-1,61-33,-16 6,40-7,75-34,-174 74,37-9,-37 12,0-2,25-10,-19 5,-1 1,2 1,44-10,-55 15,-3 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15826.33">9671 2550,'1'-2,"-1"1,1-1,-1 1,1-1,-1 1,1-1,0 1,0-1,1 1,-1 0,0-1,0 1,0 0,0 0,0 0,0 0,0 0,3-1,29-16,-29 15,47-19,52-16,-86 31,105-43,-79 30,2 3,50-13,-51 18,-2-2,0-2,51-27,-81 37,2 1,-1 1,25-5,25-7,145-80,-74 32,-121 59</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17031.64">11157 1936,'1'-1,"-1"-1,0 2,0-1,2 0,-2 0,1 0,-1-1,1 1,0 0,-1 0,1 0,0 0,0 0,-1 0,1 1,0-1,0 0,1-1,23-14,-11 8,27-18,69-33,-63 38,53-39,-70 41,2 2,48-19,-45 21,-2-1,35-22,-41 22,49-20,10-6,-34 8,-43 29</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18376.25">12312 1288,'11'-1,"1"-1,0 0,0-1,0 0,-1-1,0 0,0 0,13-8,-7 3,0 2,26-8,-12 4,-1 0,1-2,45-27,36-15,-54 28,70-42,3-4,-119 66,-2 0,2 0,13-12,-1 1,-19 14,1 1,0 0,0 0,0 1,-1 0,14-3,-13 4,1-1,-1 1,0-2,1 1,-2-1,1 1,9-7,27-20,-32 24</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20112.79">13641 622,'4'-1,"-1"0,0 0,0 0,0 0,-1-1,1 1,0-1,0 0,-2 1,3-1,-2-1,0 1,4-3,3-4,6-2,1 1,0 0,-1 1,30-11,-27 13,0-2,0 0,27-20,-24 16,1-1,45-21,-12 7,58-43,28-5,-89 50,-37 19,0 1,0-2,-2 0,1-1,-1-1,19-17,-24 21,0-1,1 1,-2 1,3-1,-2 1,17-5,21-13,-36 17,4-2,0-1,0 0,18-19,-24 21</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1621 3257,'296'0,"-282"1,-1 0,26 6,-24-4,-1 0,20 0,441-1,-232-4,-40 2,-188 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2111.37">3334 3275,'1383'0,"-1368"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3690.33">5231 3257,'1253'0,"-1237"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5880.65">6980 3239,'1193'0,"-1179"1,-2 0,27 6,14 2,-38-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8698.84">0 3239,'589'0,"-572"1,-1 0,25 6,-23-3,-1-2,22 2,13-5,-25 0,-1 1,1 1,-1 2,27 5,-25-4,2 0,-1-2,0-1,38-3,1 0,5 2,-57 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14544.8">8878 3081,'6'-1,"0"0,0 0,-1-1,1 0,-1 0,0 0,1-1,-1 1,0-1,0 0,1-1,4-5,-4 4,2 0,-2 1,1 0,0 0,1 1,6-4,23-5,-2-1,64-33,-17 6,42-8,80-33,-184 74,39-10,-39 13,0-2,26-10,-20 5,0 1,1 1,47-10,-58 15,-4 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15826.33">10186 2569,'1'-2,"-1"1,1-1,-1 1,1-1,-1 1,1-1,0 1,0-1,1 1,-1 0,0-1,0 1,0 0,0 0,1 0,-1 0,0 0,3-1,31-16,-31 15,49-19,56-17,-91 32,110-43,-82 30,1 3,53-14,-54 19,-1-2,-1-2,54-27,-85 37,1 1,0 1,26-5,26-8,153-79,-77 31,-129 60</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17031.64">11751 1951,'1'-1,"-1"-1,0 1,0 0,2 0,-2 0,1 0,-1-1,1 1,0 0,-1 0,1 0,0 0,0 0,-1 0,1 1,0-1,0 0,2-1,23-14,-11 8,28-18,73-33,-67 37,56-38,-73 41,2 2,50-20,-47 22,-2-1,36-22,-42 22,51-21,10-5,-35 8,-45 29</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18376.25">12967 1298,'12'-1,"1"-1,-1 0,1-1,-1 0,0-1,0 0,-1-1,14-7,-7 3,0 2,28-8,-14 4,0 0,0-2,48-27,38-16,-56 29,72-43,4-3,-125 66,-2 0,1 0,14-12,0 0,-21 15,1 1,1 0,-1 0,0 1,0 0,14-3,-14 4,1-1,0 1,-1-2,1 1,-1-1,0 1,10-7,28-20,-34 24</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20112.79">14367 627,'4'-1,"-1"0,1 0,-1 0,0 0,-1-1,1 1,0-1,0 0,-1 1,2-1,-2-1,0 1,4-4,4-3,6-2,0 1,1 0,-1 1,31-11,-28 13,0-2,0 0,29-20,-26 15,1 0,48-21,-14 7,63-44,28-4,-93 50,-39 19,-1 0,1-1,-2 0,1-1,-2-1,21-17,-26 21,1-1,0 1,-1 1,2-1,-1 1,17-5,22-13,-37 16,4-1,-1-1,1 0,19-19,-26 21</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1255,11 +1255,11 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1,'5'1,"-1"0,1 1,0 0,-1 0,1 0,-2 0,2 1,-1-1,0 1,5 7,3-2,308 215,-225-167,22 12,-85-46,78 47,-13-8,-45-29,68 33,-88-49,34 24,18 8,-27-25,-39-16,1 1,28 17,-25-9,-13-9,1-1,0 0,0 0,0-1,1-1,12 5,-21-9,0 1,0 0,0-1,0 1,1 0,-1 1,0-2,0 1,1 2,5 5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1441.7">1784 1000,'10'0,"-2"2,2 1,-2-1,2 1,-2 1,0 0,1 0,-1 1,9 5,10 6,222 97,-216-100,0 2,451 170,-468-180,61 16,90 41,-133-39,-29-19,4 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2595.19">3498 1700,'9'1,"2"0,-2 1,1 0,-1 0,14 6,12 3,104 24,149 40,314 73,-495-119,27 5,-113-30</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4113.38">5403 2191,'7'1,"1"0,-3 0,2 1,-1-1,0 1,1 0,-1 1,6 3,14 6,33 7,1-3,74 11,-68-15,30 6,6 1,153 46,-8 3,-230-65,4 3,0 1,0 1,23 13,-20-9,13 2,-1-1,57 11,8 2,-85-21</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5566.46">7292 2733,'44'-1,"-2"3,2 1,-1 2,49 13,385 88,-178-39,-228-45,-1 3,74 37,-11 4,-111-55,1-1,0-2,46 11,9 4,-66-19,0-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1,'5'1,"0"0,0 1,0 0,-1 0,1 0,-1 0,1 1,-1-1,0 1,6 7,2-2,325 217,-236-169,22 13,-89-47,81 48,-12-9,-49-29,73 34,-94-50,37 24,18 9,-28-26,-41-16,1 1,30 17,-27-9,-13-9,0-1,1 0,-1 0,1-1,0-1,13 5,-21-9,-1 1,0 0,0-1,0 1,1 0,-1 1,0-1,0 0,2 2,4 5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1441.7">1879 1007,'10'1,"-1"1,1 1,-1-1,1 1,-1 1,-1 0,2 0,-2 1,10 5,11 6,233 98,-228-101,1 2,475 171,-493-181,64 17,95 40,-140-39,-31-19,4 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2595.19">3684 1713,'10'1,"1"0,-1 1,0 0,0 0,14 6,13 3,109 24,158 41,330 73,-522-120,29 5,-118-30</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4113.38">5691 2207,'7'1,"1"0,-2 0,1 1,-1-1,1 2,0-1,-1 1,7 3,14 6,36 7,0-3,78 11,-72-15,32 6,7 1,160 47,-7 3,-244-66,6 3,-1 1,0 1,24 13,-20-9,12 2,0-1,60 11,9 3,-90-22</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5566.46">7680 2754,'46'-1,"-1"3,1 1,-1 2,52 13,406 88,-188-38,-241-46,0 3,78 38,-12 3,-117-55,1-1,0-1,49 10,9 4,-69-19,0-1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1286,7 +1286,7 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1505 1053,'2'-127,"-4"-139,0 255,0 0,-1-1,0 1,1 0,-3 2,0-2,1 1,-9-12,-15-40,21 45,-3 1,2 0,-2-1,-1 2,0 0,-22-22,5 5,12 14,-1 0,0 2,-38-28,-64-32,108 70,-26-15,-3 2,0 1,0 3,-1 2,-1 1,-86-14,85 19,12 1,-2 1,1 2,-57 1,79 5,2-1,-1 1,0 1,0 0,1 0,0 0,1 1,-2 0,-12 13,11-8,0-1,0 2,1 1,-12 18,-9 12,21-30,1 0,-1 0,3 2,-1-1,0 1,-6 23,-18 91,17-60,-22 125,34-154,2 47,1-53,-2 0,-6 50,-6-23,-36 98,-4 46,45-174,-2 29,1 0,3 0,2 63,5-93,2 0,1 0,1-1,11 40,46 109,-48-141,39 83,-32-72,27 74,-37-90,1-2,2 1,0-1,36 46,-2 4,-39-66,0 0,1 0,-1-1,2-1,0 1,1-3,0 2,20 11,8 2,65 31,-96-52,-1 0,0 0,1-1,-1 0,1-1,16 1,-1-2,29-3,-46 2,-1 0,0-1,0 0,0 0,0 0,-1-1,0 0,1 0,0 0,7-8,6-5,24-27,-19 19,9-11,43-61,19-22,-78 98,-1 0,-2-3,23-41,-8 15,-21 35,-1 0,0 0,-1 0,-1-1,0 0,-1 0,-2 0,1 0,2-28,2-15,1-13,-6 42,3 0,0 1,1-1,20-51,-16 53,-1-1,-1-1,-2 0,5-46,-2 14,-6 45,3-31,-6 31,3-1,0 0,2 0,0 1,6-18,-1 9,4-26,-8 30,12-34,-12 42,-1 0,0-1,-2 0,0 0,0 0,1-19,-5-178,1 196</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1585 1061,'2'-128,"-4"-140,0 257,0 0,-1-1,0 1,0 0,-2 1,0-1,1 1,-10-12,-15-40,21 45,-2 0,1 1,-1-1,-2 2,0 0,-22-22,4 4,13 15,0 0,-1 2,-40-28,-68-33,115 71,-28-15,-3 2,0 1,-1 3,0 1,-1 2,-91-14,90 19,12 1,-2 1,2 2,-61 1,84 5,1-1,0 1,-1 1,1 0,0 0,1 0,0 1,-1 0,-13 13,11-8,1 0,-1 1,2 1,-13 18,-10 12,23-30,0 0,0 1,2 1,0-1,0 1,-7 23,-19 92,19-60,-24 125,35-155,3 48,1-54,-2 0,-6 51,-7-23,-37 98,-5 46,48-175,-3 30,2-1,2 1,3 63,5-94,2 0,1 0,2 0,11 39,48 110,-50-141,40 83,-32-73,27 75,-38-91,0-2,3 2,0-2,37 46,-1 5,-42-67,1 0,0 0,0-1,2-1,-1 1,2-2,-1 1,22 11,8 2,69 31,-102-52,0 0,-1 0,2-1,-2 0,2-1,16 1,-1-2,31-3,-49 2,0 0,-1-1,0 0,1 0,-1 0,-1-1,1 0,0 0,0 0,8-8,6-5,25-27,-20 19,10-12,45-60,20-23,-82 99,-1-1,-2-2,24-41,-9 14,-21 36,-2 0,0 0,0 0,-2-1,0 0,-1 0,-1 0,0-1,2-27,2-15,2-14,-7 43,3 0,1 0,0 0,21-51,-16 52,-2 0,0-1,-3 0,5-47,-1 15,-7 45,3-32,-5 32,2-1,0 0,2 0,0 1,7-19,-2 10,5-26,-9 30,13-35,-12 43,-2 0,0-1,-2 0,1 0,-1 0,1-20,-5-178,1 197</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1615,14 +1615,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.77734375" style="6"/>
+    <col min="1" max="1" width="31.73046875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.73046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="14" t="s">
         <v>63</v>
       </c>
@@ -1633,15 +1633,15 @@
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -1659,14 +1659,14 @@
       <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="7" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>81</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Blue</v>
@@ -1757,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A16" si="1">A3</f>
         <v>Blue</v>
@@ -1788,7 +1788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Blue</v>
@@ -1819,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Blue</v>
@@ -1852,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Blue</v>
@@ -1885,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Blue</v>
@@ -1916,7 +1916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Blue</v>
@@ -1947,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Blue</v>
@@ -1978,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Blue</v>
@@ -2011,7 +2011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Blue</v>
@@ -2044,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Blue</v>
@@ -2075,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Blue</v>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Blue</v>
@@ -2137,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Blue</v>
@@ -2170,10 +2170,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I21" s="18"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B25" s="17">
         <v>1</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="17" t="s">
         <v>87</v>
       </c>
@@ -2210,22 +2210,22 @@
       <selection pane="bottomLeft" activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="3"/>
-    <col min="2" max="2" width="12.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="3"/>
+    <col min="2" max="2" width="12.796875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.53125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.265625" style="3" customWidth="1"/>
     <col min="7" max="7" width="43" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="3" customWidth="1"/>
-    <col min="9" max="12" width="8.77734375" style="1"/>
-    <col min="13" max="13" width="11.44140625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.77734375" style="1"/>
+    <col min="8" max="8" width="10.9296875" style="3" customWidth="1"/>
+    <col min="9" max="12" width="8.796875" style="1"/>
+    <col min="13" max="13" width="11.46484375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -2258,7 +2258,7 @@
       </c>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Red</v>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A70" si="1">A3</f>
         <v>Red</v>
@@ -2347,7 +2347,7 @@
       </c>
       <c r="L4" s="9"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2376,7 +2376,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2405,7 +2405,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2434,7 +2434,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2469,7 +2469,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2498,7 +2498,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2530,7 +2530,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2559,7 +2559,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2588,7 +2588,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2617,7 +2617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2646,7 +2646,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2675,7 +2675,7 @@
         <v>0.85000000000000009</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2707,7 +2707,7 @@
         <v>0.25000000000000011</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2742,7 +2742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2771,7 +2771,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2801,7 +2801,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2830,7 +2830,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2859,7 +2859,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2894,7 +2894,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2923,7 +2923,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A24" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2952,7 +2952,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A25" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2984,7 +2984,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3019,7 +3019,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A27" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3051,7 +3051,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A28" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3083,7 +3083,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A29" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3115,7 +3115,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A30" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3147,7 +3147,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A31" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3179,7 +3179,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A32" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3211,7 +3211,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3243,7 +3243,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A34" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3275,7 +3275,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3307,7 +3307,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3342,7 +3342,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A37" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3374,7 +3374,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Red</v>
@@ -3406,7 +3406,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A39" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3438,7 +3438,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A40" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3470,7 +3470,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A41" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3502,7 +3502,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A42" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3534,7 +3534,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A43" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3566,7 +3566,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A44" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3598,7 +3598,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A45" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3630,7 +3630,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3665,7 +3665,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A47" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3697,7 +3697,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A48" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3729,7 +3729,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A49" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3764,7 +3764,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A50" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3793,7 +3793,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A51" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3822,7 +3822,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A52" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3851,7 +3851,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A53" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3883,7 +3883,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A54" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3912,7 +3912,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A55" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3941,7 +3941,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A56" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3970,7 +3970,7 @@
         <v>-0.8660000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A57" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3999,7 +3999,7 @@
         <v>-0.4910000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A58" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4028,7 +4028,7 @@
         <v>-0.1160000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A59" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4057,7 +4057,7 @@
         <v>0.6339999999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A60" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4086,7 +4086,7 @@
         <v>1.0089999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A61" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4121,7 +4121,7 @@
         <v>1.0089999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A62" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4150,7 +4150,7 @@
         <v>0.6339999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A63" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4179,7 +4179,7 @@
         <v>-0.1160000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A64" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4208,7 +4208,7 @@
         <v>-0.8660000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A65" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4237,7 +4237,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A66" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4266,7 +4266,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A67" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4295,7 +4295,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A68" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4327,7 +4327,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A69" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4359,7 +4359,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A70" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -4391,7 +4391,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A71" s="3" t="str">
         <f t="shared" ref="A71:A134" si="5">A70</f>
         <v>Red</v>
@@ -4423,7 +4423,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A72" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -4455,7 +4455,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A73" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -4487,7 +4487,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A74" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -4519,7 +4519,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A75" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -4551,7 +4551,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A76" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -4583,7 +4583,7 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A77" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -4615,538 +4615,538 @@
         <v>-1.2410000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A78" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C78" s="5"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A79" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C79" s="5"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A80" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C80" s="5"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A81" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C81" s="5"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A82" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C82" s="5"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A83" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C83" s="5"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A84" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C84" s="5"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A85" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C85" s="5"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A86" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C86" s="5"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A87" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C87" s="5"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A88" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C88" s="5"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A89" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C89" s="5"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A90" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A91" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C91" s="5"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A92" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C92" s="5"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A93" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C93" s="5"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A94" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C94" s="5"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A95" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C95" s="5"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A96" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C96" s="5"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A97" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C97" s="5"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A98" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C98" s="5"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A99" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C99" s="5"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A100" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C100" s="5"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A101" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C101" s="5"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A102" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C102" s="5"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A103" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C103" s="5"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A104" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C104" s="5"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A105" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C105" s="5"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A106" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C106" s="5"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A107" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C107" s="5"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A108" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C108" s="5"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A109" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C109" s="5"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A110" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C110" s="5"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A111" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C111" s="5"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A112" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C112" s="5"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A113" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C113" s="5"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A114" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C114" s="5"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A115" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C115" s="5"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A116" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C116" s="5"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A117" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C117" s="5"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A118" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C118" s="5"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A119" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C119" s="5"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A120" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C120" s="5"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A121" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C121" s="5"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A122" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C122" s="5"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A123" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C123" s="5"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A124" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C124" s="5"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A125" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C125" s="5"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A126" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C126" s="5"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A127" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C127" s="5"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A128" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C128" s="5"/>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A129" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C129" s="5"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A130" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C130" s="5"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A131" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C131" s="5"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A132" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C132" s="5"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A133" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C133" s="5"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A134" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C134" s="5"/>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A135" s="3" t="str">
         <f t="shared" ref="A135:A154" si="6">A134</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C135" s="5"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A136" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C136" s="5"/>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A137" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C137" s="5"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A138" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C138" s="5"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A139" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C139" s="5"/>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A140" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C140" s="5"/>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A141" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C141" s="5"/>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A142" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C142" s="5"/>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A143" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C143" s="5"/>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A144" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C144" s="5"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A145" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C145" s="5"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A146" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C146" s="5"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A147" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C147" s="5"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A148" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C148" s="5"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A149" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C149" s="5"/>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A150" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C150" s="5"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A151" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C151" s="5"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A152" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C152" s="5"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A153" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C153" s="5"/>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A154" s="3" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
@@ -5168,22 +5168,22 @@
       <selection pane="bottomLeft" activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="3"/>
-    <col min="2" max="2" width="12.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="3"/>
+    <col min="2" max="2" width="12.796875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.53125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.265625" style="3" customWidth="1"/>
     <col min="7" max="7" width="31" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" style="3"/>
-    <col min="9" max="12" width="8.77734375" style="1"/>
-    <col min="13" max="13" width="11.44140625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.77734375" style="1"/>
+    <col min="8" max="8" width="8.796875" style="3"/>
+    <col min="9" max="12" width="8.796875" style="1"/>
+    <col min="13" max="13" width="11.46484375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Green</v>
@@ -5289,7 +5289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A70" si="2">A3</f>
         <v>Green</v>
@@ -5323,7 +5323,7 @@
       </c>
       <c r="L4" s="9"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5356,7 +5356,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5389,7 +5389,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5422,7 +5422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5456,7 +5456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5489,7 +5489,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5528,7 +5528,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5561,7 +5561,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5594,7 +5594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5630,7 +5630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A14" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5663,7 +5663,7 @@
         <v>7.7142857142857153</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A15" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5696,7 +5696,7 @@
         <v>7.7142857142857153</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A16" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5729,7 +5729,7 @@
         <v>7.7142857142857153</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A17" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5768,7 +5768,7 @@
         <v>7.7142857142857153</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A18" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5801,7 +5801,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A19" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5834,7 +5834,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5870,7 +5870,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A21" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5903,7 +5903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A22" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5936,7 +5936,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5975,7 +5975,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A24" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6008,7 +6008,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A25" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6041,7 +6041,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A26" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6074,7 +6074,7 @@
         <v>10.285714285714286</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A27" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6107,7 +6107,7 @@
         <v>5.1428571428571432</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A28" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6140,7 +6140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A29" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6173,7 +6173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A30" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6209,7 +6209,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A31" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6242,7 +6242,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A32" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6281,7 +6281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A33" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6314,7 +6314,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A34" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6347,7 +6347,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A35" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6380,7 +6380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A36" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6413,7 +6413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A37" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6449,7 +6449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Green</v>
@@ -6485,7 +6485,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A39" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6521,7 +6521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A40" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6560,7 +6560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A41" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6596,7 +6596,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A42" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6632,7 +6632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A43" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6668,7 +6668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A44" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6704,7 +6704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A45" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6740,7 +6740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A46" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6776,7 +6776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A47" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6812,7 +6812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A48" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6848,7 +6848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A49" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6887,7 +6887,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A50" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6923,7 +6923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A51" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6959,7 +6959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A52" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -6995,7 +6995,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A53" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7031,7 +7031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A54" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7067,7 +7067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A55" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7103,7 +7103,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A56" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7139,7 +7139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A57" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7175,7 +7175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A58" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7214,7 +7214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A59" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7250,7 +7250,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A60" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7283,7 +7283,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A61" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7316,7 +7316,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A62" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7349,7 +7349,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A63" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7385,7 +7385,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A64" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7418,7 +7418,7 @@
         <v>5.1428571428571432</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A65" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7451,7 +7451,7 @@
         <v>5.1428571428571432</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A66" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7490,7 +7490,7 @@
         <v>10.285714285714286</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A67" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7523,7 +7523,7 @@
         <v>10.285714285714286</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A68" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7556,7 +7556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A69" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7589,7 +7589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A70" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -7622,7 +7622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A71" s="3" t="str">
         <f t="shared" ref="A71:A134" si="7">A70</f>
         <v>Green</v>
@@ -7655,7 +7655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A72" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7688,7 +7688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A73" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7721,7 +7721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A74" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7760,7 +7760,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A75" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7793,7 +7793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A76" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7826,7 +7826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A77" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7862,7 +7862,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A78" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7901,7 +7901,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A79" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7934,7 +7934,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A80" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -7967,7 +7967,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A81" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8000,7 +8000,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A82" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8033,7 +8033,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A83" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8066,7 +8066,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A84" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8099,7 +8099,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A85" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8132,7 +8132,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A86" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8168,7 +8168,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A87" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8201,7 +8201,7 @@
         <v>14.399999999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A88" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8234,7 +8234,7 @@
         <v>12.470399999999998</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A89" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8273,7 +8273,7 @@
         <v>14.399999999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A90" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8306,7 +8306,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A91" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8339,7 +8339,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A92" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8372,7 +8372,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A93" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8405,7 +8405,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A94" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8438,7 +8438,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A95" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8471,7 +8471,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A96" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8504,7 +8504,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A97" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8543,7 +8543,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A98" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8576,7 +8576,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A99" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8609,7 +8609,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A100" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8642,7 +8642,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A101" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8675,7 +8675,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A102" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8708,7 +8708,7 @@
         <v>4.8461538461538467</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A103" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8741,7 +8741,7 @@
         <v>12.857142857142859</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A104" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8774,7 +8774,7 @@
         <v>12.857142857142859</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A105" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8807,7 +8807,7 @@
         <v>10.285714285714286</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A106" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8847,7 +8847,7 @@
         <v>12.857142857142859</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A107" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8880,7 +8880,7 @@
         <v>12.857142857142859</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A108" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8913,7 +8913,7 @@
         <v>11.571428571428573</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A109" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8946,7 +8946,7 @@
         <v>12.857142857142859</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A110" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -8979,7 +8979,7 @@
         <v>12.857142857142859</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A111" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9012,7 +9012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A112" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9045,7 +9045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A113" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9078,7 +9078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A114" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9111,7 +9111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A115" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9152,7 +9152,7 @@
         <v>19.439999999999998</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A116" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9185,7 +9185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A117" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9218,7 +9218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A118" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9251,7 +9251,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A119" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9284,7 +9284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A120" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9317,7 +9317,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A121" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9350,7 +9350,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A122" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9383,7 +9383,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A123" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9419,7 +9419,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A124" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9459,7 +9459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A125" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9495,7 +9495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A126" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9531,7 +9531,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A127" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9567,7 +9567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A128" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9603,7 +9603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A129" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9639,7 +9639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A130" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9675,7 +9675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A131" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9711,7 +9711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A132" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9747,7 +9747,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A133" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9787,7 +9787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A134" s="3" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -9823,7 +9823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A135" s="3" t="str">
         <f t="shared" ref="A135:A151" si="13">A134</f>
         <v>Green</v>
@@ -9859,7 +9859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A136" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -9895,7 +9895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A137" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -9931,7 +9931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A138" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -9967,7 +9967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A139" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10003,7 +10003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A140" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10039,7 +10039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A141" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10075,7 +10075,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A142" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10115,7 +10115,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A143" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10151,7 +10151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A144" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10187,7 +10187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A145" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10220,7 +10220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A146" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10253,7 +10253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A147" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10286,7 +10286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A148" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10319,7 +10319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A149" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10353,7 +10353,7 @@
         <v>33.119999999999997</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A150" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10386,7 +10386,7 @@
         <v>7.1999999999999993</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A151" s="3" t="str">
         <f t="shared" si="13"/>
         <v>Green</v>
@@ -10419,13 +10419,13 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K153" s="1">
         <f>MIN(K2:K151)</f>
         <v>4.8461538461538467</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K154" s="1">
         <f>K153/1.2</f>
         <v>4.0384615384615392</v>
@@ -10444,9 +10444,9 @@
       <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A1" s="20" t="s">
         <v>17</v>
       </c>
@@ -10462,7 +10462,7 @@
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
     </row>
-    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>16</v>
       </c>
@@ -10476,16 +10476,16 @@
       <c r="I2" s="19"/>
       <c r="J2" s="19"/>
     </row>
-    <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.4" x14ac:dyDescent="0.45">
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15.4" x14ac:dyDescent="0.45">
       <c r="E9" s="10"/>
     </row>
-    <row r="19" spans="11:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="11:11" ht="15.4" x14ac:dyDescent="0.45">
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="11:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="11:11" ht="15.4" x14ac:dyDescent="0.45">
       <c r="K20" s="10"/>
     </row>
   </sheetData>
@@ -10506,7 +10506,7 @@
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10519,7 +10519,7 @@
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>